<commit_message>
save nssec and llti maps and commentary
</commit_message>
<xml_diff>
--- a/tables/proportion_ranks.xlsx
+++ b/tables/proportion_ranks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="car_rank_change" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="pensioner_rank_change" sheetId="10" r:id="rId10"/>
     <sheet name="religious_rank_change" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -192,7 +192,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -242,7 +242,7 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2598,8 +2598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7754,7 +7754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -8785,8 +8785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="Q48" sqref="Q48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9814,10 +9814,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9828,7 +9828,7 @@
     <col min="6" max="6" width="7.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>48</v>
       </c>
@@ -9844,7 +9844,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2">
         <v>2001</v>
@@ -9860,7 +9860,7 @@
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -9879,8 +9879,12 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <f>IF(C3&gt;0.5, 1, 0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -9899,8 +9903,12 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H4">
+        <f t="shared" ref="H4:H50" si="0">IF(C4&gt;0.5, 1, 0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -9919,8 +9927,12 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -9939,8 +9951,12 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -9959,8 +9975,12 @@
       <c r="F7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -9979,8 +9999,12 @@
       <c r="F8">
         <v>-1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -9999,8 +10023,12 @@
       <c r="F9">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -10019,8 +10047,12 @@
       <c r="F10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -10039,8 +10071,12 @@
       <c r="F11">
         <v>-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -10059,8 +10095,12 @@
       <c r="F12">
         <v>-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -10079,8 +10119,12 @@
       <c r="F13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -10099,8 +10143,12 @@
       <c r="F14">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -10119,8 +10167,12 @@
       <c r="F15">
         <v>-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -10139,8 +10191,12 @@
       <c r="F16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -10159,8 +10215,12 @@
       <c r="F17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -10179,8 +10239,12 @@
       <c r="F18">
         <v>-5</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -10199,8 +10263,12 @@
       <c r="F19">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -10219,8 +10287,12 @@
       <c r="F20">
         <v>-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -10239,8 +10311,12 @@
       <c r="F21">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -10259,8 +10335,12 @@
       <c r="F22">
         <v>-7</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -10279,8 +10359,12 @@
       <c r="F23">
         <v>-9</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -10299,8 +10383,12 @@
       <c r="F24">
         <v>-1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -10319,8 +10407,12 @@
       <c r="F25">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -10339,8 +10431,12 @@
       <c r="F26">
         <v>-5</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -10359,8 +10455,12 @@
       <c r="F27">
         <v>-10</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -10379,8 +10479,12 @@
       <c r="F28">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -10399,8 +10503,12 @@
       <c r="F29">
         <v>-1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -10419,8 +10527,12 @@
       <c r="F30">
         <v>-1</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -10439,8 +10551,12 @@
       <c r="F31">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -10459,8 +10575,12 @@
       <c r="F32">
         <v>-6</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -10479,8 +10599,12 @@
       <c r="F33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -10499,8 +10623,12 @@
       <c r="F34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -10519,8 +10647,12 @@
       <c r="F35">
         <v>-5</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -10539,8 +10671,12 @@
       <c r="F36">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>21</v>
       </c>
@@ -10559,8 +10695,12 @@
       <c r="F37">
         <v>-5</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -10579,8 +10719,12 @@
       <c r="F38">
         <v>-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -10599,8 +10743,12 @@
       <c r="F39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>16</v>
       </c>
@@ -10619,8 +10767,12 @@
       <c r="F40">
         <v>-9</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -10639,8 +10791,12 @@
       <c r="F41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>28</v>
       </c>
@@ -10659,8 +10815,12 @@
       <c r="F42">
         <v>-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -10679,8 +10839,12 @@
       <c r="F43">
         <v>-1</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H43">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -10699,8 +10863,12 @@
       <c r="F44">
         <v>-7</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -10719,8 +10887,12 @@
       <c r="F45">
         <v>-4</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -10739,8 +10911,12 @@
       <c r="F46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H46">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -10759,8 +10935,12 @@
       <c r="F47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -10779,8 +10959,12 @@
       <c r="F48">
         <v>-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -10799,8 +10983,12 @@
       <c r="F49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>38</v>
       </c>
@@ -10818,6 +11006,20 @@
       </c>
       <c r="F50">
         <v>0</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H51">
+        <f>SUM(H3:H50)</f>
+        <v>25</v>
+      </c>
+      <c r="I51">
+        <f>H51/48</f>
+        <v>0.52083333333333337</v>
       </c>
     </row>
   </sheetData>
@@ -10849,7 +11051,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
reach end of stage 1 of report - descriptive stats
</commit_message>
<xml_diff>
--- a/tables/proportion_ranks.xlsx
+++ b/tables/proportion_ranks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9396" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="car_rank_change" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,16 @@
     <sheet name="marstat_rank_change" sheetId="8" r:id="rId8"/>
     <sheet name="nsssec_rank_change" sheetId="9" r:id="rId9"/>
     <sheet name="pensioner_rank_change" sheetId="10" r:id="rId10"/>
-    <sheet name="religious_rank_change" sheetId="11" r:id="rId11"/>
+    <sheet name="student_rank_change" sheetId="12" r:id="rId11"/>
+    <sheet name="religious_rank_change" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="52">
   <si>
     <t>Glasgow</t>
   </si>
@@ -240,10 +242,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -548,23 +552,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="A2" s="6"/>
       <c r="B2">
         <v>2001</v>
       </c>
@@ -577,7 +581,7 @@
       <c r="E2">
         <v>2011</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -1567,8 +1571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1580,23 +1584,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="A2" s="6"/>
       <c r="B2">
         <v>2001</v>
       </c>
@@ -1609,7 +1613,7 @@
       <c r="E2">
         <v>2011</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -2598,8 +2602,1040 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2">
+        <v>2001</v>
+      </c>
+      <c r="C2">
+        <v>2011</v>
+      </c>
+      <c r="D2">
+        <v>2001</v>
+      </c>
+      <c r="E2">
+        <v>2011</v>
+      </c>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.99379335523914E-2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>6.0406289676726198E-2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.6357166352680801E-2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.24165272227142E-2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.25179808716468E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1.86983099604459E-2</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.1278022936351301E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.67223495250923E-2</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>8.7331355315456508E-3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.08535282446114E-2</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6.6044321979970497E-3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.30136179017693E-2</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2.36189476446661E-3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4.1895683591497901E-3</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>8.8280503510448298E-4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5.8842254526512798E-4</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1">
+        <v>7.5120192307692301E-4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.6280016280016301E-3</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1">
+        <v>6.3900238173615002E-4</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.9354949214668701E-3</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4.8344898191332E-4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1.6655823031880301E-3</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4.4452763090168903E-4</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3.9239537758245199E-4</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <v>24</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2.4227740763173799E-4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2.0565552699228801E-4</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>31</v>
+      </c>
+      <c r="F15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2.14059422895796E-4</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6.2837584897588105E-4</v>
+      </c>
+      <c r="D16">
+        <v>14</v>
+      </c>
+      <c r="E16">
+        <v>19</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.08805631786183E-4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3.3552092979560099E-4</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>26</v>
+      </c>
+      <c r="F17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2.0020020020019999E-4</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3.72925601342532E-4</v>
+      </c>
+      <c r="D18">
+        <v>16</v>
+      </c>
+      <c r="E18">
+        <v>25</v>
+      </c>
+      <c r="F18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.9767868741351599E-4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.99690479756378E-4</v>
+      </c>
+      <c r="D19">
+        <v>17</v>
+      </c>
+      <c r="E19">
+        <v>32</v>
+      </c>
+      <c r="F19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.9504583577140599E-4</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2.0135456708768101E-3</v>
+      </c>
+      <c r="D20">
+        <v>18</v>
+      </c>
+      <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.8446781036709101E-4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1.6903313049357701E-4</v>
+      </c>
+      <c r="D21">
+        <v>19</v>
+      </c>
+      <c r="E21">
+        <v>35</v>
+      </c>
+      <c r="F21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1.7842804888928499E-4</v>
+      </c>
+      <c r="C22" s="3">
+        <v>7.1564885496183195E-4</v>
+      </c>
+      <c r="D22" s="4">
+        <v>20</v>
+      </c>
+      <c r="E22" s="4">
+        <v>17</v>
+      </c>
+      <c r="F22">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.46412884333821E-4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>5.28157390902489E-4</v>
+      </c>
+      <c r="D23">
+        <v>21</v>
+      </c>
+      <c r="E23">
+        <v>22</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.3279330721731601E-4</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1.24649423496416E-4</v>
+      </c>
+      <c r="D24">
+        <v>22</v>
+      </c>
+      <c r="E24">
+        <v>38</v>
+      </c>
+      <c r="F24">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1.30872922392357E-4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1.14238386953976E-4</v>
+      </c>
+      <c r="D25">
+        <v>23</v>
+      </c>
+      <c r="E25">
+        <v>39</v>
+      </c>
+      <c r="F25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1.2605571662674899E-4</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2.3795359904818601E-4</v>
+      </c>
+      <c r="D26">
+        <v>24</v>
+      </c>
+      <c r="E26">
+        <v>29</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1.17841150129625E-4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1.3308195630475799E-3</v>
+      </c>
+      <c r="D27">
+        <v>25</v>
+      </c>
+      <c r="E27">
+        <v>13</v>
+      </c>
+      <c r="F27">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1.12650670271488E-4</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1.0417751849151E-4</v>
+      </c>
+      <c r="D28">
+        <v>26</v>
+      </c>
+      <c r="E28">
+        <v>40</v>
+      </c>
+      <c r="F28">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1.10803324099723E-4</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1.00502512562814E-4</v>
+      </c>
+      <c r="D29">
+        <v>27</v>
+      </c>
+      <c r="E29">
+        <v>42</v>
+      </c>
+      <c r="F29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1.02212909490469E-4</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1.27394620762138E-4</v>
+      </c>
+      <c r="D30">
+        <v>28</v>
+      </c>
+      <c r="E30">
+        <v>37</v>
+      </c>
+      <c r="F30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.01853738032186E-4</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2.5710363572087699E-4</v>
+      </c>
+      <c r="D31">
+        <v>29</v>
+      </c>
+      <c r="E31">
+        <v>28</v>
+      </c>
+      <c r="F31">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="1">
+        <v>9.3181013436702097E-5</v>
+      </c>
+      <c r="C32" s="1">
+        <v>4.8225629427611701E-4</v>
+      </c>
+      <c r="D32">
+        <v>30</v>
+      </c>
+      <c r="E32">
+        <v>23</v>
+      </c>
+      <c r="F32">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="1">
+        <v>8.6303616121515504E-5</v>
+      </c>
+      <c r="C33" s="1">
+        <v>6.58616904500549E-4</v>
+      </c>
+      <c r="D33">
+        <v>31</v>
+      </c>
+      <c r="E33">
+        <v>18</v>
+      </c>
+      <c r="F33">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1">
+        <v>8.0528265421162803E-5</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1.8401295451199801E-4</v>
+      </c>
+      <c r="D34">
+        <v>32</v>
+      </c>
+      <c r="E34">
+        <v>34</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="1">
+        <v>5.62793707966345E-5</v>
+      </c>
+      <c r="C35" s="1">
+        <v>5.63322578993189E-4</v>
+      </c>
+      <c r="D35">
+        <v>33</v>
+      </c>
+      <c r="E35">
+        <v>21</v>
+      </c>
+      <c r="F35">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>41</v>
+      </c>
+      <c r="E36">
+        <v>45.5</v>
+      </c>
+      <c r="F36">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>41</v>
+      </c>
+      <c r="E37">
+        <v>45.5</v>
+      </c>
+      <c r="F37">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2.1321961620469101E-4</v>
+      </c>
+      <c r="D38">
+        <v>41</v>
+      </c>
+      <c r="E38">
+        <v>30</v>
+      </c>
+      <c r="F38">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1.30718954248366E-3</v>
+      </c>
+      <c r="D39">
+        <v>41</v>
+      </c>
+      <c r="E39">
+        <v>14</v>
+      </c>
+      <c r="F39">
+        <v>-27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2.8500855025650801E-4</v>
+      </c>
+      <c r="D40">
+        <v>41</v>
+      </c>
+      <c r="E40">
+        <v>27</v>
+      </c>
+      <c r="F40">
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1.0334849111203E-4</v>
+      </c>
+      <c r="D41">
+        <v>41</v>
+      </c>
+      <c r="E41">
+        <v>41</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1.3764624913971101E-4</v>
+      </c>
+      <c r="D42">
+        <v>41</v>
+      </c>
+      <c r="E42">
+        <v>36</v>
+      </c>
+      <c r="F42">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1.8575276307235101E-4</v>
+      </c>
+      <c r="D43">
+        <v>41</v>
+      </c>
+      <c r="E43">
+        <v>33</v>
+      </c>
+      <c r="F43">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1.9721577726218098E-3</v>
+      </c>
+      <c r="D44">
+        <v>41</v>
+      </c>
+      <c r="E44">
+        <v>9</v>
+      </c>
+      <c r="F44">
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>41</v>
+      </c>
+      <c r="E45">
+        <v>45.5</v>
+      </c>
+      <c r="F45">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>41</v>
+      </c>
+      <c r="E46">
+        <v>45.5</v>
+      </c>
+      <c r="F46">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1.24688279301746E-3</v>
+      </c>
+      <c r="D47">
+        <v>41</v>
+      </c>
+      <c r="E47">
+        <v>15</v>
+      </c>
+      <c r="F47">
+        <v>-26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>41</v>
+      </c>
+      <c r="E48">
+        <v>45.5</v>
+      </c>
+      <c r="F48">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1.2456747404844301E-3</v>
+      </c>
+      <c r="D49">
+        <v>41</v>
+      </c>
+      <c r="E49">
+        <v>16</v>
+      </c>
+      <c r="F49">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>41</v>
+      </c>
+      <c r="E50">
+        <v>45.5</v>
+      </c>
+      <c r="F50">
+        <v>4.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F3:F50">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2611,23 +3647,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="A2" s="6"/>
       <c r="B2">
         <v>2001</v>
       </c>
@@ -2640,7 +3676,7 @@
       <c r="E2">
         <v>2011</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -3642,23 +4678,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="A2" s="6"/>
       <c r="B2">
         <v>2001</v>
       </c>
@@ -3671,7 +4707,7 @@
       <c r="E2">
         <v>2011</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -4673,23 +5709,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="A2" s="6"/>
       <c r="B2">
         <v>2001</v>
       </c>
@@ -4702,7 +5738,7 @@
       <c r="E2">
         <v>2011</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -5705,23 +6741,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="A2" s="6"/>
       <c r="B2">
         <v>2001</v>
       </c>
@@ -5734,7 +6770,7 @@
       <c r="E2">
         <v>2011</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -6736,23 +7772,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="A2" s="6"/>
       <c r="B2">
         <v>2001</v>
       </c>
@@ -6765,7 +7801,7 @@
       <c r="E2">
         <v>2011</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -7767,23 +8803,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="A2" s="6"/>
       <c r="B2">
         <v>2001</v>
       </c>
@@ -7796,7 +8832,7 @@
       <c r="E2">
         <v>2011</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -8798,23 +9834,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="A2" s="6"/>
       <c r="B2">
         <v>2001</v>
       </c>
@@ -8827,7 +9863,7 @@
       <c r="E2">
         <v>2011</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -9829,23 +10865,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="A2" s="6"/>
       <c r="B2">
         <v>2001</v>
       </c>
@@ -9858,7 +10894,7 @@
       <c r="E2">
         <v>2011</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -11063,23 +12099,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
+      <c r="A2" s="6"/>
       <c r="B2">
         <v>2001</v>
       </c>
@@ -11092,7 +12128,7 @@
       <c r="E2">
         <v>2011</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">

</xml_diff>